<commit_message>
Final submission for pcmlai capstone with additional models
</commit_message>
<xml_diff>
--- a/Data/MultiShopFailures.xlsx
+++ b/Data/MultiShopFailures.xlsx
@@ -463,7 +463,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2022 Jeep Grand</t>
+          <t>2022 Jeep Grand Cherokee Enhanced Powertrain</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -481,7 +481,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2022 Jeep Grand</t>
+          <t>2022 Jeep Grand Cherokee Enhanced Powertrain</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -499,7 +499,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2021 Jeep Grand</t>
+          <t>2021 Jeep Grand Cherokee Enhanced Powertrain</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -517,7 +517,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2021 Jeep Grand</t>
+          <t>2021 Jeep Grand Cherokee Enhanced Powertrain</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -535,7 +535,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2021 Jeep Grand</t>
+          <t>2021 Jeep Grand Cherokee Enhanced Powertrain</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -553,7 +553,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024 Jeep Grand</t>
+          <t>2024 Jeep Grand Wagoneer L Enhanced Powertrain</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -571,7 +571,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024 Jeep Wagoneer</t>
+          <t>2024 Jeep Wagoneer Enhanced Powertrain</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -589,7 +589,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024 Jeep Wagoneer</t>
+          <t>2024 Jeep Wagoneer Enhanced Powertrain</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -607,7 +607,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024 Dodge Ram</t>
+          <t>2024 Dodge Ram 1500 Enhanced Powertrain</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -625,7 +625,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2023 Dodge Ram</t>
+          <t>2023 Dodge Ram 1500 Enhanced Powertrain</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -643,7 +643,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2017 Jeep Compass</t>
+          <t>2017 Jeep Compass Enhanced Powertrain</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -661,7 +661,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024 Chevrolet Blazer</t>
+          <t>2024 Chevrolet Blazer Enhanced Powertrain</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -679,7 +679,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2017 Kia Forte</t>
+          <t>2017 Kia Forte 4 Door Enhanced Powertrain UDS - Theta GDI 1.6 / 2.0L</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -697,7 +697,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2020 Toyota RAV4</t>
+          <t>2020 Toyota RAV4 Enhanced Powertrain CAN</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -715,7 +715,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2006 Subaru Outback</t>
+          <t>2006 Subaru Outback Enhanced Powertrain</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -733,7 +733,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2018 Hyundai Santa</t>
+          <t>2018 Hyundai Santa Fe 2.4L Enhanced Powertrain UDS - Theta 2.XL</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -751,7 +751,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2017 Hyundai Santa</t>
+          <t>2017 Hyundai Santa Fe 2.4L Enhanced Powertrain UDS - Theta 2.XL</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -769,7 +769,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2018 Hyundai Santa</t>
+          <t>2018 Hyundai Santa Fe 2.4L Enhanced Powertrain UDS - Theta 2.XL</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -787,7 +787,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2018 Hyundai Santa</t>
+          <t>2018 Hyundai Santa Fe 2.4L Enhanced Powertrain UDS - Theta 2.XL</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -805,7 +805,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2017 Hyundai Santa</t>
+          <t>2017 Hyundai Santa Fe 2.4L Enhanced Powertrain UDS - Theta 2.XL</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -823,7 +823,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2017 Hyundai Santa</t>
+          <t>2017 Hyundai Santa Fe 2.4L Enhanced Powertrain UDS - Theta 2.XL</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -841,7 +841,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2017 Hyundai Santa</t>
+          <t>2017 Hyundai Santa Fe 2.4L Enhanced Powertrain UDS - Theta 2.XL</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -859,7 +859,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2017 Hyundai Santa</t>
+          <t>2017 Hyundai Santa Fe 2.4L Enhanced Powertrain UDS - Theta 2.XL</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -877,7 +877,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2017 Hyundai Santa</t>
+          <t>2017 Hyundai Santa Fe 2.4L Enhanced Powertrain UDS - Theta 2.XL</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -895,7 +895,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2020 Volvo S60</t>
+          <t>2020 Volvo S60 Engine Control Module (ECM)</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -913,7 +913,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024 Mitsubishi Outlander</t>
+          <t>2024 Mitsubishi Outlander PHEV Enhanced Powertrain CAN</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -931,7 +931,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024 Mitsubishi Outlander</t>
+          <t>2024 Mitsubishi Outlander PHEV Enhanced Powertrain CAN</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -949,7 +949,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2024 Mitsubishi Outlander</t>
+          <t>2024 Mitsubishi Outlander PHEV Enhanced Powertrain CAN</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -967,7 +967,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2022 Subaru Impreza</t>
+          <t>2022 Subaru Impreza Enhanced Powertrain CAN</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -985,7 +985,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2023 Subaru Impreza</t>
+          <t>2023 Subaru Impreza Enhanced Powertrain CAN</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2024 Alfa-Romeo Stelvio</t>
+          <t>2024 Alfa-Romeo Stelvio Enhanced Powertrain</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2019 Toyota Corolla</t>
+          <t>2019 Toyota Corolla Enhanced Powertrain CAN</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2022 Hyundai Kona</t>
+          <t>2022 Hyundai Kona Enhanced Powertrain UDS - T-GDI 1.6L Gamma</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1057,7 +1057,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2023 Hyundai Kona</t>
+          <t>2023 Hyundai Kona Enhanced Powertrain UDS - T-GDI 1.6L Gamma</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2022 Hyundai Kona</t>
+          <t>2022 Hyundai Kona Enhanced Powertrain UDS - MPI 2.0L</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2023 Hyundai Kona</t>
+          <t>2023 Hyundai Kona Enhanced Powertrain UDS - T-GDI 1.6L Gamma</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1111,7 +1111,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2019 Volvo XC60</t>
+          <t>2019 Volvo XC60 Engine Control Module (ECM)</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1129,7 +1129,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2024 Mercedes-Benz C</t>
+          <t>2024 Mercedes-Benz C Class Enhanced Powertrain CAN MED41</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1147,7 +1147,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2007 BMW 3</t>
+          <t>2007 BMW 3 Series Enhanced Powertrain</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2009 Volvo S40</t>
+          <t>2009 Volvo S40 Enhanced Powertrain CAN</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2023 Volvo XC90</t>
+          <t>2023 Volvo XC90 Engine Control Module (ECM)</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2019 Volvo XC40</t>
+          <t>2019 Volvo XC40 Supplemental Restraint System Module (SRS)</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1219,7 +1219,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2018 Volvo XC90</t>
+          <t>2018 Volvo XC90 Engine Control Module (ECM)</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1237,7 +1237,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2019 Volvo XC90</t>
+          <t>2019 Volvo XC90 Engine Control Module (ECM)</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2017 Volvo XC90</t>
+          <t>2017 Volvo XC90 Engine Control Module (ECM)</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2019 Volvo XC90</t>
+          <t>2019 Volvo XC90 Engine Control Module (ECM)</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2016 Volvo XC90</t>
+          <t>2016 Volvo XC90 Engine Control Module (ECM)</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2022 Volvo XC90</t>
+          <t>2022 Volvo XC90 Engine Control Module (ECM)</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1327,7 +1327,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2017 Volvo XC90</t>
+          <t>2017 Volvo XC90 Engine Control Module (ECM)</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1345,7 +1345,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2018 Volvo XC90</t>
+          <t>2018 Volvo XC90 Engine Control Module (ECM)</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2019 Volvo XC90</t>
+          <t>2019 Volvo XC90 Engine Control Module (ECM)</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2018 Volvo XC60</t>
+          <t>2018 Volvo XC60 Supplemental Restraint System Module (SRS)</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1399,7 +1399,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2021 Volvo XC60</t>
+          <t>2021 Volvo XC60 Engine Control Module (ECM)</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2019 Dodge Ram</t>
+          <t>2019 Dodge Ram 1500 Enhanced Powertrain</t>
         </is>
       </c>
       <c r="C55" t="n">

</xml_diff>